<commit_message>
- fixed issue where wrong delta was used when only deltaInDays was 0 - dates are now differently interpolated to fix issues with 28.2/29.2 as intermediate date - all tests pass
</commit_message>
<xml_diff>
--- a/exampleCSV/autoFill.xlsx
+++ b/exampleCSV/autoFill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janis/Documents/Projects/Web/vscode-edit-csv/exampleCSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3043F693-15FF-494E-840C-8CF8DF7A8F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7215C1-AFF6-004A-964E-FF4B65144422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="620" windowWidth="36380" windowHeight="22980" xr2:uid="{A4F2C004-9924-234E-A009-8AD0C35DE3FA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26340" windowHeight="25740" xr2:uid="{A4F2C004-9924-234E-A009-8AD0C35DE3FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="222">
   <si>
     <t>2 2</t>
   </si>
@@ -751,6 +751,84 @@
   </si>
   <si>
     <t>different day (delta != 0) -&gt; use constant delta days</t>
+  </si>
+  <si>
+    <t>delta 11 months</t>
+  </si>
+  <si>
+    <t>delta 1 month</t>
+  </si>
+  <si>
+    <t>delta 13 months</t>
+  </si>
+  <si>
+    <t>delta 23 months</t>
+  </si>
+  <si>
+    <t>test 30.12.2020</t>
+  </si>
+  <si>
+    <t>test 30.01.2021</t>
+  </si>
+  <si>
+    <t>test 30.12.2021</t>
+  </si>
+  <si>
+    <t>test 30.01.2022</t>
+  </si>
+  <si>
+    <t>test 30.12.2022</t>
+  </si>
+  <si>
+    <t>1 30.12.2020</t>
+  </si>
+  <si>
+    <t>2 30.01.2021</t>
+  </si>
+  <si>
+    <t>2 30.12.2020</t>
+  </si>
+  <si>
+    <t>3 30.01.2021</t>
+  </si>
+  <si>
+    <t>3 30.12.2020</t>
+  </si>
+  <si>
+    <t>4 30.01.2021</t>
+  </si>
+  <si>
+    <t>anders (no sequence?)</t>
+  </si>
+  <si>
+    <t>30.12.2020 30.12.2020</t>
+  </si>
+  <si>
+    <t>30.01.2021 30.01.2021</t>
+  </si>
+  <si>
+    <t>30.12.2020 30.12.2021</t>
+  </si>
+  <si>
+    <t>30.01.2021 30.01.2022</t>
+  </si>
+  <si>
+    <t>30.12.2020 30.12.2022</t>
+  </si>
+  <si>
+    <t>30.01.2021 30.01.2023</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
   </si>
 </sst>
 </file>
@@ -811,7 +889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -825,6 +903,7 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1210,15 +1289,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037C1F4-3E38-A146-9ED5-F06910296F22}">
-  <dimension ref="B6:AU111"/>
+  <dimension ref="B6:AU113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z51" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AJ74" sqref="AJ74"/>
+    <sheetView tabSelected="1" topLeftCell="Z66" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AI101" sqref="AI101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="35" max="35" width="16" customWidth="1"/>
+    <col min="35" max="35" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:35" x14ac:dyDescent="0.2">
@@ -3274,7 +3353,7 @@
     </row>
     <row r="64" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U64">
-        <f>W64-W63</f>
+        <f t="shared" ref="U64:U90" si="0">W64-W63</f>
         <v>366</v>
       </c>
       <c r="W64" s="12">
@@ -3288,14 +3367,14 @@
         <v>44198</v>
       </c>
       <c r="AB64">
-        <f>AA64-AA63</f>
+        <f t="shared" ref="AB64:AB90" si="1">AA64-AA63</f>
         <v>367</v>
       </c>
       <c r="AG64" s="12">
         <v>44562</v>
       </c>
       <c r="AI64">
-        <f>AJ64-AJ63</f>
+        <f t="shared" ref="AI64:AI90" si="2">AJ64-AJ63</f>
         <v>60</v>
       </c>
       <c r="AJ64" s="12">
@@ -3325,7 +3404,7 @@
     </row>
     <row r="65" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U65">
-        <f>W65-W64</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W65" s="3">
@@ -3339,18 +3418,18 @@
         <v>44565</v>
       </c>
       <c r="AB65">
-        <f>AA65-AA64</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF65">
-        <f>AG64-AG63</f>
+        <f t="shared" ref="AF65:AF90" si="3">AG64-AG63</f>
         <v>731</v>
       </c>
       <c r="AG65" s="3">
         <v>45292</v>
       </c>
       <c r="AI65">
-        <f>AJ65-AJ64</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ65" s="3">
@@ -3360,27 +3439,27 @@
         <v>44686</v>
       </c>
       <c r="AN65">
-        <f t="shared" ref="AN65:AN80" si="0">AM65-AM64</f>
+        <f t="shared" ref="AN65:AN80" si="4">AM65-AM64</f>
         <v>426</v>
       </c>
       <c r="AQ65" s="12">
         <v>44748</v>
       </c>
       <c r="AR65">
-        <f t="shared" ref="AR65:AR82" si="1">AQ65-AQ64</f>
+        <f t="shared" ref="AR65:AR82" si="5">AQ65-AQ64</f>
         <v>459</v>
       </c>
       <c r="AT65" s="12">
         <v>44593</v>
       </c>
       <c r="AU65">
-        <f t="shared" ref="AU65:AU83" si="2">AT65-AT64</f>
+        <f t="shared" ref="AU65:AU83" si="6">AT65-AT64</f>
         <v>396</v>
       </c>
     </row>
     <row r="66" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U66">
-        <f>W66-W65</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W66" s="3">
@@ -3394,18 +3473,18 @@
         <v>44932</v>
       </c>
       <c r="AB66">
-        <f>AA66-AA65</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF66">
-        <f>AG65-AG64</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG66" s="3">
         <v>46023</v>
       </c>
       <c r="AI66">
-        <f>AJ66-AJ65</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ66" s="3">
@@ -3415,27 +3494,27 @@
         <v>45112</v>
       </c>
       <c r="AN66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>426</v>
       </c>
       <c r="AQ66" s="3">
         <v>43831</v>
       </c>
       <c r="AR66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-917</v>
       </c>
       <c r="AT66" s="3">
         <v>43831</v>
       </c>
       <c r="AU66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-762</v>
       </c>
     </row>
     <row r="67" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U67">
-        <f>W67-W66</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W67" s="3">
@@ -3445,18 +3524,18 @@
         <v>45299</v>
       </c>
       <c r="AB67">
-        <f>AA67-AA66</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF67">
-        <f>AG66-AG65</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG67" s="3">
         <v>46753</v>
       </c>
       <c r="AI67">
-        <f>AJ67-AJ66</f>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="AJ67" s="3">
@@ -3466,27 +3545,27 @@
         <v>45540</v>
       </c>
       <c r="AN67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>428</v>
       </c>
       <c r="AQ67" s="3">
         <v>44289</v>
       </c>
       <c r="AR67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>458</v>
       </c>
       <c r="AT67" s="3">
         <v>44197</v>
       </c>
       <c r="AU67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>366</v>
       </c>
     </row>
     <row r="68" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U68">
-        <f>W68-W67</f>
+        <f t="shared" si="0"/>
         <v>366</v>
       </c>
       <c r="W68" s="3">
@@ -3496,18 +3575,18 @@
         <v>45666</v>
       </c>
       <c r="AB68">
-        <f>AA68-AA67</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF68">
-        <f>AG67-AG66</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG68" s="3">
         <v>47484</v>
       </c>
       <c r="AI68">
-        <f>AJ68-AJ67</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ68" s="3">
@@ -3517,27 +3596,27 @@
         <v>45966</v>
       </c>
       <c r="AN68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>426</v>
       </c>
       <c r="AQ68" s="3">
         <v>44748</v>
       </c>
       <c r="AR68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>459</v>
       </c>
       <c r="AT68" s="3">
         <v>44593</v>
       </c>
       <c r="AU68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>396</v>
       </c>
     </row>
     <row r="69" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U69">
-        <f>W69-W68</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W69" s="3">
@@ -3547,18 +3626,18 @@
         <v>46033</v>
       </c>
       <c r="AB69">
-        <f>AA69-AA68</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF69">
-        <f>AG68-AG67</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG69" s="3">
         <v>48214</v>
       </c>
       <c r="AI69">
-        <f>AJ69-AJ68</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ69" s="3">
@@ -3568,27 +3647,27 @@
         <v>46392</v>
       </c>
       <c r="AN69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>426</v>
       </c>
       <c r="AQ69" s="3">
         <v>43831</v>
       </c>
       <c r="AR69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-917</v>
       </c>
       <c r="AT69" s="3">
         <v>43831</v>
       </c>
       <c r="AU69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-762</v>
       </c>
     </row>
     <row r="70" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U70">
-        <f>W70-W69</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W70" s="3">
@@ -3598,18 +3677,18 @@
         <v>46400</v>
       </c>
       <c r="AB70">
-        <f>AA70-AA69</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF70">
-        <f>AG69-AG68</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG70" s="3">
         <v>48945</v>
       </c>
       <c r="AI70">
-        <f>AJ70-AJ69</f>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="AJ70" s="3">
@@ -3619,27 +3698,27 @@
         <v>46817</v>
       </c>
       <c r="AN70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>425</v>
       </c>
       <c r="AQ70" s="3">
         <v>44289</v>
       </c>
       <c r="AR70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>458</v>
       </c>
       <c r="AT70" s="3">
         <v>44197</v>
       </c>
       <c r="AU70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>366</v>
       </c>
     </row>
     <row r="71" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U71">
-        <f>W71-W70</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W71" s="3">
@@ -3649,18 +3728,18 @@
         <v>46767</v>
       </c>
       <c r="AB71">
-        <f>AA71-AA70</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF71">
-        <f>AG70-AG69</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG71" s="3">
         <v>49675</v>
       </c>
       <c r="AI71">
-        <f>AJ71-AJ70</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ71" s="3">
@@ -3670,27 +3749,27 @@
         <v>47243</v>
       </c>
       <c r="AN71">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>426</v>
       </c>
       <c r="AQ71" s="3">
         <v>44748</v>
       </c>
       <c r="AR71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>459</v>
       </c>
       <c r="AT71" s="3">
         <v>44593</v>
       </c>
       <c r="AU71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>396</v>
       </c>
     </row>
     <row r="72" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U72">
-        <f>W72-W71</f>
+        <f t="shared" si="0"/>
         <v>366</v>
       </c>
       <c r="W72" s="3">
@@ -3700,18 +3779,18 @@
         <v>47134</v>
       </c>
       <c r="AB72">
-        <f>AA72-AA71</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF72">
-        <f>AG71-AG70</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG72" s="3">
         <v>50406</v>
       </c>
       <c r="AI72">
-        <f>AJ72-AJ71</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ72" s="3">
@@ -3721,27 +3800,27 @@
         <v>47669</v>
       </c>
       <c r="AN72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>426</v>
       </c>
       <c r="AQ72" s="3">
         <v>43831</v>
       </c>
       <c r="AR72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-917</v>
       </c>
       <c r="AT72" s="3">
         <v>43831</v>
       </c>
       <c r="AU72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-762</v>
       </c>
     </row>
     <row r="73" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U73">
-        <f>W73-W72</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W73" s="3">
@@ -3751,18 +3830,18 @@
         <v>47501</v>
       </c>
       <c r="AB73">
-        <f>AA73-AA72</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF73">
-        <f>AG72-AG71</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG73" s="3">
         <v>51136</v>
       </c>
       <c r="AI73">
-        <f>AJ73-AJ72</f>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="AJ73" s="3">
@@ -3772,27 +3851,27 @@
         <v>48096</v>
       </c>
       <c r="AN73">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>427</v>
       </c>
       <c r="AQ73" s="3">
         <v>44289</v>
       </c>
       <c r="AR73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>458</v>
       </c>
       <c r="AT73" s="3">
         <v>44197</v>
       </c>
       <c r="AU73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>366</v>
       </c>
     </row>
     <row r="74" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U74">
-        <f>W74-W73</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W74" s="3">
@@ -3802,18 +3881,18 @@
         <v>47868</v>
       </c>
       <c r="AB74">
-        <f>AA74-AA73</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF74">
-        <f>AG73-AG72</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG74" s="3">
         <v>51867</v>
       </c>
       <c r="AI74">
-        <f>AJ74-AJ73</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ74" s="3">
@@ -3823,27 +3902,27 @@
         <v>48523</v>
       </c>
       <c r="AN74">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>427</v>
       </c>
       <c r="AQ74" s="3">
         <v>44748</v>
       </c>
       <c r="AR74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>459</v>
       </c>
       <c r="AT74" s="3">
         <v>44593</v>
       </c>
       <c r="AU74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>396</v>
       </c>
     </row>
     <row r="75" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U75">
-        <f>W75-W74</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W75" s="3">
@@ -3853,18 +3932,18 @@
         <v>48235</v>
       </c>
       <c r="AB75">
-        <f>AA75-AA74</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF75">
-        <f>AG74-AG73</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG75" s="3">
         <v>52597</v>
       </c>
       <c r="AI75">
-        <f>AJ75-AJ74</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ75" s="3">
@@ -3874,27 +3953,27 @@
         <v>48949</v>
       </c>
       <c r="AN75">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>426</v>
       </c>
       <c r="AQ75" s="3">
         <v>43831</v>
       </c>
       <c r="AR75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-917</v>
       </c>
       <c r="AT75" s="3">
         <v>43831</v>
       </c>
       <c r="AU75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-762</v>
       </c>
     </row>
     <row r="76" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U76">
-        <f>W76-W75</f>
+        <f t="shared" si="0"/>
         <v>366</v>
       </c>
       <c r="W76" s="3">
@@ -3904,18 +3983,18 @@
         <v>48602</v>
       </c>
       <c r="AB76">
-        <f>AA76-AA75</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF76">
-        <f>AG75-AG74</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG76" s="3">
         <v>53328</v>
       </c>
       <c r="AI76">
-        <f>AJ76-AJ75</f>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="AJ76" s="3">
@@ -3925,27 +4004,27 @@
         <v>49373</v>
       </c>
       <c r="AN76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>424</v>
       </c>
       <c r="AQ76" s="3">
         <v>44289</v>
       </c>
       <c r="AR76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>458</v>
       </c>
       <c r="AT76" s="3">
         <v>44197</v>
       </c>
       <c r="AU76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>366</v>
       </c>
     </row>
     <row r="77" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U77">
-        <f>W77-W76</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W77" s="3">
@@ -3955,18 +4034,18 @@
         <v>48969</v>
       </c>
       <c r="AB77">
-        <f>AA77-AA76</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF77">
-        <f>AG76-AG75</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG77" s="3">
         <v>54058</v>
       </c>
       <c r="AI77">
-        <f>AJ77-AJ76</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ77" s="3">
@@ -3976,27 +4055,27 @@
         <v>49800</v>
       </c>
       <c r="AN77">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>427</v>
       </c>
       <c r="AQ77" s="3">
         <v>44748</v>
       </c>
       <c r="AR77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>459</v>
       </c>
       <c r="AT77" s="3">
         <v>44593</v>
       </c>
       <c r="AU77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>396</v>
       </c>
     </row>
     <row r="78" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U78">
-        <f>W78-W77</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W78" s="3">
@@ -4006,18 +4085,18 @@
         <v>49336</v>
       </c>
       <c r="AB78">
-        <f>AA78-AA77</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF78">
-        <f>AG77-AG76</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG78" s="3">
         <v>54789</v>
       </c>
       <c r="AI78">
-        <f>AJ78-AJ77</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ78" s="3">
@@ -4027,27 +4106,27 @@
         <v>50226</v>
       </c>
       <c r="AN78">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>426</v>
       </c>
       <c r="AQ78" s="3">
         <v>43831</v>
       </c>
       <c r="AR78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-917</v>
       </c>
       <c r="AT78" s="3">
         <v>43831</v>
       </c>
       <c r="AU78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-762</v>
       </c>
     </row>
     <row r="79" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U79">
-        <f>W79-W78</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W79" s="3">
@@ -4057,18 +4136,18 @@
         <v>49703</v>
       </c>
       <c r="AB79">
-        <f>AA79-AA78</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF79">
-        <f>AG78-AG77</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG79" s="3">
         <v>55519</v>
       </c>
       <c r="AI79">
-        <f>AJ79-AJ78</f>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="AJ79" s="3">
@@ -4078,27 +4157,27 @@
         <v>50653</v>
       </c>
       <c r="AN79">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>427</v>
       </c>
       <c r="AQ79" s="3">
         <v>44289</v>
       </c>
       <c r="AR79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>458</v>
       </c>
       <c r="AT79" s="3">
         <v>44197</v>
       </c>
       <c r="AU79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>366</v>
       </c>
     </row>
     <row r="80" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U80">
-        <f>W80-W79</f>
+        <f t="shared" si="0"/>
         <v>366</v>
       </c>
       <c r="W80" s="3">
@@ -4108,18 +4187,18 @@
         <v>50070</v>
       </c>
       <c r="AB80">
-        <f>AA80-AA79</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF80">
-        <f>AG79-AG78</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG80" s="3">
         <v>56250</v>
       </c>
       <c r="AI80">
-        <f>AJ80-AJ79</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ80" s="3">
@@ -4129,27 +4208,27 @@
         <v>51079</v>
       </c>
       <c r="AN80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>426</v>
       </c>
       <c r="AQ80" s="3">
         <v>44748</v>
       </c>
       <c r="AR80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>459</v>
       </c>
       <c r="AT80" s="3">
         <v>44593</v>
       </c>
       <c r="AU80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>396</v>
       </c>
     </row>
     <row r="81" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U81">
-        <f>W81-W80</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W81" s="3">
@@ -4159,18 +4238,18 @@
         <v>50437</v>
       </c>
       <c r="AB81">
-        <f>AA81-AA80</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF81">
-        <f>AG80-AG79</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG81" s="3">
         <v>56980</v>
       </c>
       <c r="AI81">
-        <f>AJ81-AJ80</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ81" s="3">
@@ -4180,20 +4259,20 @@
         <v>43831</v>
       </c>
       <c r="AR81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-917</v>
       </c>
       <c r="AT81" s="3">
         <v>43831</v>
       </c>
       <c r="AU81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-762</v>
       </c>
     </row>
     <row r="82" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U82">
-        <f>W82-W81</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W82" s="3">
@@ -4203,18 +4282,18 @@
         <v>50804</v>
       </c>
       <c r="AB82">
-        <f>AA82-AA81</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF82">
-        <f>AG81-AG80</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG82" s="3">
         <v>57711</v>
       </c>
       <c r="AI82">
-        <f>AJ82-AJ81</f>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="AJ82" s="3">
@@ -4224,20 +4303,20 @@
         <v>44289</v>
       </c>
       <c r="AR82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>458</v>
       </c>
       <c r="AT82" s="3">
         <v>44197</v>
       </c>
       <c r="AU82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>366</v>
       </c>
     </row>
     <row r="83" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U83">
-        <f>W83-W82</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W83" s="3">
@@ -4247,18 +4326,18 @@
         <v>51171</v>
       </c>
       <c r="AB83">
-        <f>AA83-AA82</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF83">
-        <f>AG82-AG81</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG83" s="3">
         <v>58441</v>
       </c>
       <c r="AI83">
-        <f>AJ83-AJ82</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ83" s="3">
@@ -4271,13 +4350,13 @@
         <v>44593</v>
       </c>
       <c r="AU83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>396</v>
       </c>
     </row>
     <row r="84" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U84">
-        <f>W84-W83</f>
+        <f t="shared" si="0"/>
         <v>366</v>
       </c>
       <c r="W84" s="3">
@@ -4287,18 +4366,18 @@
         <v>51538</v>
       </c>
       <c r="AB84">
-        <f>AA84-AA83</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF84">
-        <f>AG83-AG82</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG84" s="3">
         <v>59172</v>
       </c>
       <c r="AI84">
-        <f>AJ84-AJ83</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ84" s="3">
@@ -4307,7 +4386,7 @@
     </row>
     <row r="85" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U85">
-        <f>W85-W84</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W85" s="3">
@@ -4317,18 +4396,18 @@
         <v>51905</v>
       </c>
       <c r="AB85">
-        <f>AA85-AA84</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF85">
-        <f>AG84-AG83</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG85" s="3">
         <v>59902</v>
       </c>
       <c r="AI85">
-        <f>AJ85-AJ84</f>
+        <f t="shared" si="2"/>
         <v>62</v>
       </c>
       <c r="AJ85" s="3">
@@ -4337,7 +4416,7 @@
     </row>
     <row r="86" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U86">
-        <f>W86-W85</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W86" s="3">
@@ -4347,18 +4426,18 @@
         <v>52272</v>
       </c>
       <c r="AB86">
-        <f>AA86-AA85</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF86">
-        <f>AG85-AG84</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG86" s="3">
         <v>60633</v>
       </c>
       <c r="AI86">
-        <f>AJ86-AJ85</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ86" s="3">
@@ -4367,7 +4446,7 @@
     </row>
     <row r="87" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U87">
-        <f>W87-W86</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W87" s="3">
@@ -4377,18 +4456,18 @@
         <v>52639</v>
       </c>
       <c r="AB87">
-        <f>AA87-AA86</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF87">
-        <f>AG86-AG85</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG87" s="3">
         <v>61363</v>
       </c>
       <c r="AI87">
-        <f>AJ87-AJ86</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ87" s="3">
@@ -4397,7 +4476,7 @@
     </row>
     <row r="88" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U88">
-        <f>W88-W87</f>
+        <f t="shared" si="0"/>
         <v>366</v>
       </c>
       <c r="W88" s="3">
@@ -4407,18 +4486,18 @@
         <v>53006</v>
       </c>
       <c r="AB88">
-        <f>AA88-AA87</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF88">
-        <f>AG87-AG86</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG88" s="3">
         <v>62094</v>
       </c>
       <c r="AI88">
-        <f>AJ88-AJ87</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="AJ88" s="3">
@@ -4427,7 +4506,7 @@
     </row>
     <row r="89" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U89">
-        <f>W89-W88</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W89" s="3">
@@ -4437,18 +4516,18 @@
         <v>53373</v>
       </c>
       <c r="AB89">
-        <f>AA89-AA88</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF89">
-        <f>AG88-AG87</f>
+        <f t="shared" si="3"/>
         <v>731</v>
       </c>
       <c r="AG89" s="3">
         <v>62824</v>
       </c>
       <c r="AI89">
-        <f>AJ89-AJ88</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ89" s="3">
@@ -4457,7 +4536,7 @@
     </row>
     <row r="90" spans="21:47" x14ac:dyDescent="0.2">
       <c r="U90">
-        <f>W90-W89</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
       <c r="W90" s="3">
@@ -4467,18 +4546,18 @@
         <v>53740</v>
       </c>
       <c r="AB90">
-        <f>AA90-AA89</f>
+        <f t="shared" si="1"/>
         <v>367</v>
       </c>
       <c r="AF90">
-        <f>AG89-AG88</f>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="AG90" s="3">
         <v>63555</v>
       </c>
       <c r="AI90">
-        <f>AJ90-AJ89</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="AJ90" s="3">
@@ -4494,85 +4573,369 @@
       <c r="W96" s="3">
         <v>45292</v>
       </c>
-    </row>
-    <row r="97" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA96" t="s">
+        <v>197</v>
+      </c>
+      <c r="AC96" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF96" t="s">
+        <v>196</v>
+      </c>
+      <c r="AI96" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="97" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W97" s="3">
         <v>46753</v>
       </c>
-    </row>
-    <row r="98" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA97" s="12">
+        <v>44195</v>
+      </c>
+      <c r="AC97" s="12">
+        <v>44195</v>
+      </c>
+      <c r="AF97" s="12">
+        <v>44012</v>
+      </c>
+      <c r="AI97" s="12">
+        <v>44012</v>
+      </c>
+      <c r="AL97" s="3">
+        <v>44165</v>
+      </c>
+    </row>
+    <row r="98" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W98" s="3">
         <v>48214</v>
       </c>
-    </row>
-    <row r="99" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA98" s="12">
+        <v>44226</v>
+      </c>
+      <c r="AC98" s="12">
+        <v>44591</v>
+      </c>
+      <c r="AF98" s="12">
+        <v>44346</v>
+      </c>
+      <c r="AG98">
+        <f>AF98-AF97</f>
+        <v>334</v>
+      </c>
+      <c r="AI98" s="12">
+        <v>44711</v>
+      </c>
+      <c r="AL98" s="3">
+        <v>44165</v>
+      </c>
+    </row>
+    <row r="99" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W99" s="3">
         <v>49675</v>
       </c>
-    </row>
-    <row r="100" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA99" s="3">
+        <v>44255</v>
+      </c>
+      <c r="AC99" s="3">
+        <v>44985</v>
+      </c>
+      <c r="AD99">
+        <f>AC98-AC97</f>
+        <v>396</v>
+      </c>
+      <c r="AF99" s="3">
+        <v>44681</v>
+      </c>
+      <c r="AG99">
+        <f t="shared" ref="AG99:AG104" si="7">AF99-AF98</f>
+        <v>335</v>
+      </c>
+      <c r="AI99" s="3">
+        <v>45412</v>
+      </c>
+      <c r="AJ99">
+        <f>AI98-AI97</f>
+        <v>699</v>
+      </c>
+      <c r="AL99" s="3">
+        <v>44165</v>
+      </c>
+    </row>
+    <row r="100" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W100" s="3">
         <v>51136</v>
       </c>
-    </row>
-    <row r="101" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA100" s="3">
+        <v>44285</v>
+      </c>
+      <c r="AC100" s="3">
+        <v>45381</v>
+      </c>
+      <c r="AD100">
+        <f t="shared" ref="AD100:AD104" si="8">AC99-AC98</f>
+        <v>394</v>
+      </c>
+      <c r="AF100" s="3">
+        <v>45015</v>
+      </c>
+      <c r="AG100">
+        <f t="shared" si="7"/>
+        <v>334</v>
+      </c>
+      <c r="AI100" s="3">
+        <v>46111</v>
+      </c>
+      <c r="AJ100">
+        <f t="shared" ref="AJ100:AJ103" si="9">AI99-AI98</f>
+        <v>701</v>
+      </c>
+      <c r="AL100" s="3">
+        <v>44165</v>
+      </c>
+    </row>
+    <row r="101" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W101" s="3">
         <v>52597</v>
       </c>
-    </row>
-    <row r="102" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA101" s="3">
+        <v>44316</v>
+      </c>
+      <c r="AC101" s="3">
+        <v>45777</v>
+      </c>
+      <c r="AD101">
+        <f t="shared" si="8"/>
+        <v>396</v>
+      </c>
+      <c r="AF101" s="3">
+        <v>45351</v>
+      </c>
+      <c r="AG101">
+        <f t="shared" si="7"/>
+        <v>336</v>
+      </c>
+      <c r="AI101" s="3">
+        <v>46812</v>
+      </c>
+      <c r="AJ101">
+        <f t="shared" si="9"/>
+        <v>699</v>
+      </c>
+      <c r="AL101" s="3">
+        <v>44165</v>
+      </c>
+    </row>
+    <row r="102" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W102" s="3">
         <v>54058</v>
       </c>
-    </row>
-    <row r="103" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA102" s="3">
+        <v>44346</v>
+      </c>
+      <c r="AC102" s="3">
+        <v>46172</v>
+      </c>
+      <c r="AD102">
+        <f t="shared" si="8"/>
+        <v>396</v>
+      </c>
+      <c r="AF102" s="3">
+        <v>45687</v>
+      </c>
+      <c r="AG102">
+        <f t="shared" si="7"/>
+        <v>336</v>
+      </c>
+      <c r="AI102" s="3">
+        <v>47513</v>
+      </c>
+      <c r="AJ102">
+        <f t="shared" si="9"/>
+        <v>701</v>
+      </c>
+      <c r="AL102" s="3">
+        <v>44165</v>
+      </c>
+    </row>
+    <row r="103" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W103" s="3">
         <v>55519</v>
       </c>
-    </row>
-    <row r="104" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA103" s="3">
+        <v>44377</v>
+      </c>
+      <c r="AC103" s="3">
+        <v>46568</v>
+      </c>
+      <c r="AD103">
+        <f t="shared" si="8"/>
+        <v>395</v>
+      </c>
+      <c r="AF103" s="3">
+        <v>46021</v>
+      </c>
+      <c r="AG103">
+        <f t="shared" si="7"/>
+        <v>334</v>
+      </c>
+      <c r="AI103" s="3">
+        <v>48212</v>
+      </c>
+      <c r="AJ103">
+        <f t="shared" si="9"/>
+        <v>701</v>
+      </c>
+      <c r="AL103" s="3"/>
+    </row>
+    <row r="104" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W104" s="3">
         <v>56980</v>
       </c>
-    </row>
-    <row r="105" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA104" s="3">
+        <v>44407</v>
+      </c>
+      <c r="AC104" s="3">
+        <v>46964</v>
+      </c>
+      <c r="AD104">
+        <f t="shared" si="8"/>
+        <v>396</v>
+      </c>
+      <c r="AF104" s="3">
+        <v>46356</v>
+      </c>
+      <c r="AG104">
+        <f t="shared" si="7"/>
+        <v>335</v>
+      </c>
+      <c r="AI104" s="3">
+        <v>48913</v>
+      </c>
+      <c r="AJ104">
+        <f>AI103-AI102</f>
+        <v>699</v>
+      </c>
+      <c r="AL104" s="3"/>
+    </row>
+    <row r="105" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W105" s="3">
         <v>58441</v>
       </c>
-    </row>
-    <row r="106" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AL105" s="3"/>
+    </row>
+    <row r="106" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W106" s="3">
         <v>59902</v>
       </c>
-    </row>
-    <row r="107" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AL106" s="3"/>
+    </row>
+    <row r="107" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W107" s="3">
         <v>61363</v>
       </c>
-    </row>
-    <row r="108" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AC107" t="s">
+        <v>211</v>
+      </c>
+      <c r="AJ107" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="AL107">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="108" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W108" s="3">
         <v>62824</v>
       </c>
-    </row>
-    <row r="109" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA108" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC108" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE108" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="AJ108" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="109" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W109" s="3">
         <v>64285</v>
       </c>
-    </row>
-    <row r="110" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA109" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC109" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE109" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="AJ109" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="110" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W110" s="3">
         <v>65746</v>
       </c>
-    </row>
-    <row r="111" spans="23:23" x14ac:dyDescent="0.2">
+      <c r="AA110" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AC110" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AE110" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="AJ110" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="111" spans="23:38" x14ac:dyDescent="0.2">
       <c r="W111" s="3">
         <v>67207</v>
+      </c>
+      <c r="AA111" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC111" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="AE111" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AJ111" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="23:38" x14ac:dyDescent="0.2">
+      <c r="AA112" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC112" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE112" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="113" spans="27:31" x14ac:dyDescent="0.2">
+      <c r="AA113" s="3"/>
+      <c r="AC113" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="AE113" s="3" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>